<commit_message>
Add a2 & bp to Excel
</commit_message>
<xml_diff>
--- a/Steel Full.xlsx
+++ b/Steel Full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mousavi\Documents\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD2F994-277B-4580-8757-A7EFB2C975A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A032F40-8828-46FC-AB59-3E4428CF79D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="603" activeTab="3" xr2:uid="{F9827B19-5E74-4F5B-B072-D384967EA338}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="603" xr2:uid="{F9827B19-5E74-4F5B-B072-D384967EA338}"/>
   </bookViews>
   <sheets>
     <sheet name="IPE" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="IPB" sheetId="3" r:id="rId3"/>
     <sheet name="UNP" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="74">
   <si>
     <t>IPE</t>
   </si>
@@ -816,6 +817,44 @@
   <si>
     <t>فاصله مرکز برش تا مرکز سطح</t>
   </si>
+  <si>
+    <t>فاصله مرکز دو پروفیل برای مقطع  دوبل تقویت شده با ورق</t>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+  </si>
+  <si>
+    <t>طول ورق برای مقطع دوبل تقویت شده با ورق</t>
+  </si>
 </sst>
 </file>
 
@@ -1050,13 +1089,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1379,11 +1418,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB10F132-7E44-405D-B662-30727D902CE6}">
-  <dimension ref="A1:AE22"/>
+  <dimension ref="A1:AG22"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S29" sqref="S29"/>
+      <selection pane="bottomLeft" activeCell="U5" sqref="U5:V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1394,15 +1433,15 @@
     <col min="14" max="14" width="10.44140625" customWidth="1"/>
     <col min="17" max="17" width="10.109375" customWidth="1"/>
     <col min="18" max="18" width="10.21875" customWidth="1"/>
-    <col min="20" max="20" width="13" customWidth="1"/>
-    <col min="24" max="24" width="9.5546875" customWidth="1"/>
+    <col min="20" max="22" width="13" customWidth="1"/>
+    <col min="26" max="26" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:33" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
@@ -1458,34 +1497,40 @@
         <v>28</v>
       </c>
       <c r="U1" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="W1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="24" t="s">
+      <c r="X1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="24" t="s">
+      <c r="Y1" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="24" t="s">
+      <c r="Z1" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="25" t="s">
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="25" t="s">
+      <c r="AD1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="25" t="s">
+      <c r="AE1" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
     </row>
-    <row r="2" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+    <row r="2" spans="1:33" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1541,42 +1586,48 @@
         <v>45</v>
       </c>
       <c r="U2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="X2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="Y2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="Z2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="AA2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="14" t="s">
+      <c r="AB2" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="15" t="s">
+      <c r="AC2" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="AB2" s="15" t="s">
+      <c r="AD2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="AC2" s="15" t="s">
+      <c r="AE2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" s="15" t="s">
+      <c r="AF2" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="AE2" s="15" t="s">
+      <c r="AG2" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
+    <row r="3" spans="1:33" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1632,40 +1683,46 @@
         <v>3</v>
       </c>
       <c r="U3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="V3" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="W3" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="X3" s="14" t="s">
         <v>54</v>
       </c>
       <c r="Y3" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z3" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="14" t="s">
+      <c r="AB3" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="AA3" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB3" s="15" t="s">
-        <v>54</v>
       </c>
       <c r="AC3" s="15" t="s">
         <v>54</v>
       </c>
       <c r="AD3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AE3" s="15" t="s">
+      <c r="AG3" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="28"/>
       <c r="B4" s="28"/>
       <c r="C4" s="16"/>
@@ -1687,22 +1744,24 @@
       <c r="S4" s="16"/>
       <c r="T4" s="16"/>
       <c r="U4" s="16"/>
-      <c r="V4" s="27" t="s">
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27" t="s">
+      <c r="Y4" s="29"/>
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="29"/>
     </row>
-    <row r="5" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
         <v>8</v>
       </c>
@@ -1761,43 +1820,45 @@
       <c r="T5" s="4">
         <v>63</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4">
         <v>12.2</v>
       </c>
-      <c r="V5" s="7">
+      <c r="X5" s="7">
         <v>2400</v>
       </c>
-      <c r="W5" s="7">
+      <c r="Y5" s="7">
         <v>3700</v>
       </c>
-      <c r="X5" s="14">
+      <c r="Z5" s="14">
         <f>2.04*10^6</f>
         <v>2040000</v>
       </c>
-      <c r="Y5" s="7">
+      <c r="AA5" s="7">
         <v>54.1</v>
       </c>
-      <c r="Z5" s="7">
+      <c r="AB5" s="7">
         <v>267.2</v>
       </c>
-      <c r="AA5" s="15">
+      <c r="AC5" s="15">
         <v>3600</v>
       </c>
-      <c r="AB5" s="15">
+      <c r="AD5" s="15">
         <v>5200</v>
       </c>
-      <c r="AC5" s="15">
+      <c r="AE5" s="15">
         <f>2.04*10^6</f>
         <v>2040000</v>
       </c>
-      <c r="AD5" s="15">
+      <c r="AF5" s="15">
         <v>44.2</v>
       </c>
-      <c r="AE5" s="15">
+      <c r="AG5" s="15">
         <v>184.9</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
         <v>10</v>
       </c>
@@ -1856,43 +1917,45 @@
       <c r="T6" s="4">
         <v>79</v>
       </c>
-      <c r="U6" s="4">
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4">
         <v>14.6</v>
       </c>
-      <c r="V6" s="7">
+      <c r="X6" s="7">
         <v>2400</v>
       </c>
-      <c r="W6" s="7">
+      <c r="Y6" s="7">
         <v>3700</v>
       </c>
-      <c r="X6" s="14">
+      <c r="Z6" s="14">
         <f>2.04*10^6</f>
         <v>2040000</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="AA6" s="7">
         <v>63.8</v>
       </c>
-      <c r="Z6" s="7">
+      <c r="AB6" s="7">
         <v>276.3</v>
       </c>
-      <c r="AA6" s="15">
+      <c r="AC6" s="15">
         <v>3600</v>
       </c>
-      <c r="AB6" s="15">
+      <c r="AD6" s="15">
         <v>5200</v>
       </c>
-      <c r="AC6" s="15">
+      <c r="AE6" s="15">
         <f>2.04*10^6</f>
         <v>2040000</v>
       </c>
-      <c r="AD6" s="15">
+      <c r="AF6" s="15">
         <v>52.1</v>
       </c>
-      <c r="AE6" s="15">
+      <c r="AG6" s="15">
         <v>194.9</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
         <v>12</v>
       </c>
@@ -1951,43 +2014,45 @@
       <c r="T7" s="4">
         <v>96</v>
       </c>
-      <c r="U7" s="4">
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4">
         <v>16.899999999999999</v>
       </c>
-      <c r="V7" s="7">
+      <c r="X7" s="7">
         <v>2400</v>
       </c>
-      <c r="W7" s="7">
+      <c r="Y7" s="7">
         <v>3700</v>
       </c>
-      <c r="X7" s="14">
-        <f t="shared" ref="X7:X22" si="0">2.04*10^6</f>
-        <v>2040000</v>
-      </c>
-      <c r="Y7" s="7">
+      <c r="Z7" s="14">
+        <f t="shared" ref="Z7:Z22" si="0">2.04*10^6</f>
+        <v>2040000</v>
+      </c>
+      <c r="AA7" s="7">
         <v>74.3</v>
       </c>
-      <c r="Z7" s="7">
+      <c r="AB7" s="7">
         <v>300</v>
       </c>
-      <c r="AA7" s="15">
+      <c r="AC7" s="15">
         <v>3600</v>
       </c>
-      <c r="AB7" s="15">
+      <c r="AD7" s="15">
         <v>5200</v>
       </c>
-      <c r="AC7" s="15">
-        <f t="shared" ref="AC7:AC22" si="1">2.04*10^6</f>
-        <v>2040000</v>
-      </c>
-      <c r="AD7" s="15">
+      <c r="AE7" s="15">
+        <f t="shared" ref="AE7:AE22" si="1">2.04*10^6</f>
+        <v>2040000</v>
+      </c>
+      <c r="AF7" s="15">
         <v>60.7</v>
       </c>
-      <c r="AE7" s="15">
+      <c r="AG7" s="15">
         <v>214.5</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>14</v>
       </c>
@@ -2046,43 +2111,45 @@
       <c r="T8" s="4">
         <v>112</v>
       </c>
-      <c r="U8" s="4">
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4">
         <v>19.3</v>
       </c>
-      <c r="V8" s="7">
+      <c r="X8" s="7">
         <v>2400</v>
       </c>
-      <c r="W8" s="7">
+      <c r="Y8" s="7">
         <v>3700</v>
       </c>
-      <c r="X8" s="14">
+      <c r="Z8" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y8" s="7">
+      <c r="AA8" s="7">
         <v>84.9</v>
       </c>
-      <c r="Z8" s="7">
+      <c r="AB8" s="7">
         <v>325.7</v>
       </c>
-      <c r="AA8" s="15">
+      <c r="AC8" s="15">
         <v>3600</v>
       </c>
-      <c r="AB8" s="15">
+      <c r="AD8" s="15">
         <v>5200</v>
       </c>
-      <c r="AC8" s="15">
+      <c r="AE8" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD8" s="15">
+      <c r="AF8" s="15">
         <v>69.3</v>
       </c>
-      <c r="AE8" s="15">
+      <c r="AG8" s="15">
         <v>235.4</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>16</v>
       </c>
@@ -2141,43 +2208,45 @@
       <c r="T9" s="4">
         <v>129</v>
       </c>
-      <c r="U9" s="4">
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4">
         <v>21.7</v>
       </c>
-      <c r="V9" s="7">
+      <c r="X9" s="7">
         <v>2400</v>
       </c>
-      <c r="W9" s="7">
+      <c r="Y9" s="7">
         <v>3700</v>
       </c>
-      <c r="X9" s="14">
+      <c r="Z9" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="AA9" s="7">
         <v>94.6</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="AB9" s="7">
         <v>345.4</v>
       </c>
-      <c r="AA9" s="15">
+      <c r="AC9" s="15">
         <v>3600</v>
       </c>
-      <c r="AB9" s="15">
+      <c r="AD9" s="15">
         <v>5200</v>
       </c>
-      <c r="AC9" s="15">
+      <c r="AE9" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD9" s="15">
+      <c r="AF9" s="15">
         <v>77.2</v>
       </c>
-      <c r="AE9" s="15">
+      <c r="AG9" s="15">
         <v>252.6</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>18</v>
       </c>
@@ -2236,43 +2305,45 @@
       <c r="T10" s="4">
         <v>145</v>
       </c>
-      <c r="U10" s="4">
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4">
         <v>24</v>
       </c>
-      <c r="V10" s="7">
+      <c r="X10" s="7">
         <v>2400</v>
       </c>
-      <c r="W10" s="7">
+      <c r="Y10" s="7">
         <v>3700</v>
       </c>
-      <c r="X10" s="14">
+      <c r="Z10" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y10" s="7">
+      <c r="AA10" s="7">
         <v>105.5</v>
       </c>
-      <c r="Z10" s="7">
+      <c r="AB10" s="7">
         <v>373.4</v>
       </c>
-      <c r="AA10" s="15">
+      <c r="AC10" s="15">
         <v>3600</v>
       </c>
-      <c r="AB10" s="15">
+      <c r="AD10" s="15">
         <v>5200</v>
       </c>
-      <c r="AC10" s="15">
+      <c r="AE10" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD10" s="15">
+      <c r="AF10" s="15">
         <v>86.1</v>
       </c>
-      <c r="AE10" s="15">
+      <c r="AG10" s="15">
         <v>274.89999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
         <v>20</v>
       </c>
@@ -2331,43 +2402,45 @@
       <c r="T11" s="4">
         <v>162</v>
       </c>
-      <c r="U11" s="4">
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4">
         <v>26.4</v>
       </c>
-      <c r="V11" s="7">
+      <c r="X11" s="7">
         <v>2400</v>
       </c>
-      <c r="W11" s="7">
+      <c r="Y11" s="7">
         <v>3700</v>
       </c>
-      <c r="X11" s="14">
+      <c r="Z11" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y11" s="7">
+      <c r="AA11" s="7">
         <v>114.5</v>
       </c>
-      <c r="Z11" s="7">
+      <c r="AB11" s="7">
         <v>393.6</v>
       </c>
-      <c r="AA11" s="15">
+      <c r="AC11" s="15">
         <v>3600</v>
       </c>
-      <c r="AB11" s="15">
+      <c r="AD11" s="15">
         <v>5200</v>
       </c>
-      <c r="AC11" s="15">
+      <c r="AE11" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD11" s="15">
+      <c r="AF11" s="15">
         <v>93.5</v>
       </c>
-      <c r="AE11" s="15">
+      <c r="AG11" s="15">
         <v>292.2</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
         <v>22</v>
       </c>
@@ -2426,43 +2499,45 @@
       <c r="T12" s="4">
         <v>179</v>
       </c>
-      <c r="U12" s="4">
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4">
         <v>29.1</v>
       </c>
-      <c r="V12" s="7">
+      <c r="X12" s="7">
         <v>2400</v>
       </c>
-      <c r="W12" s="7">
+      <c r="Y12" s="7">
         <v>3700</v>
       </c>
-      <c r="X12" s="14">
+      <c r="Z12" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y12" s="7">
+      <c r="AA12" s="7">
         <v>127.1</v>
       </c>
-      <c r="Z12" s="7">
+      <c r="AB12" s="7">
         <v>430.9</v>
       </c>
-      <c r="AA12" s="15">
+      <c r="AC12" s="15">
         <v>3600</v>
       </c>
-      <c r="AB12" s="15">
+      <c r="AD12" s="15">
         <v>5200</v>
       </c>
-      <c r="AC12" s="15">
+      <c r="AE12" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD12" s="15">
+      <c r="AF12" s="15">
         <v>103.8</v>
       </c>
-      <c r="AE12" s="15">
+      <c r="AG12" s="15">
         <v>320.8</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
         <v>24</v>
       </c>
@@ -2521,43 +2596,45 @@
       <c r="T13" s="4">
         <v>196</v>
       </c>
-      <c r="U13" s="4">
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4">
         <v>31.8</v>
       </c>
-      <c r="V13" s="7">
+      <c r="X13" s="7">
         <v>2400</v>
       </c>
-      <c r="W13" s="7">
+      <c r="Y13" s="7">
         <v>3700</v>
       </c>
-      <c r="X13" s="14">
+      <c r="Z13" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y13" s="7">
+      <c r="AA13" s="7">
         <v>138.30000000000001</v>
       </c>
-      <c r="Z13" s="7">
+      <c r="AB13" s="7">
         <v>458.6</v>
       </c>
-      <c r="AA13" s="15">
+      <c r="AC13" s="15">
         <v>3600</v>
       </c>
-      <c r="AB13" s="15">
+      <c r="AD13" s="15">
         <v>5200</v>
       </c>
-      <c r="AC13" s="15">
+      <c r="AE13" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD13" s="15">
+      <c r="AF13" s="15">
         <v>112.9</v>
       </c>
-      <c r="AE13" s="15">
+      <c r="AG13" s="15">
         <v>343.2</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="28">
         <v>27</v>
       </c>
@@ -2616,43 +2693,45 @@
       <c r="T14" s="4">
         <v>220</v>
       </c>
-      <c r="U14" s="4">
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4">
         <v>35.6</v>
       </c>
-      <c r="V14" s="7">
+      <c r="X14" s="7">
         <v>2400</v>
       </c>
-      <c r="W14" s="7">
+      <c r="Y14" s="7">
         <v>3700</v>
       </c>
-      <c r="X14" s="14">
+      <c r="Z14" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y14" s="7">
+      <c r="AA14" s="7">
         <v>155.19999999999999</v>
       </c>
-      <c r="Z14" s="7">
+      <c r="AB14" s="7">
         <v>497.2</v>
       </c>
-      <c r="AA14" s="15">
+      <c r="AC14" s="15">
         <v>3600</v>
       </c>
-      <c r="AB14" s="15">
+      <c r="AD14" s="15">
         <v>5200</v>
       </c>
-      <c r="AC14" s="15">
+      <c r="AE14" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD14" s="15">
+      <c r="AF14" s="15">
         <v>126.7</v>
       </c>
-      <c r="AE14" s="15">
+      <c r="AG14" s="15">
         <v>375.9</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="28">
         <v>30</v>
       </c>
@@ -2711,43 +2790,45 @@
       <c r="T15" s="4">
         <v>245</v>
       </c>
-      <c r="U15" s="4">
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4">
         <v>39.5</v>
       </c>
-      <c r="V15" s="7">
+      <c r="X15" s="7">
         <v>2400</v>
       </c>
-      <c r="W15" s="7">
+      <c r="Y15" s="7">
         <v>3700</v>
       </c>
-      <c r="X15" s="14">
+      <c r="Z15" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y15" s="7">
+      <c r="AA15" s="7">
         <v>171.9</v>
       </c>
-      <c r="Z15" s="7">
+      <c r="AB15" s="7">
         <v>539.79999999999995</v>
       </c>
-      <c r="AA15" s="15">
+      <c r="AC15" s="15">
         <v>3600</v>
       </c>
-      <c r="AB15" s="15">
+      <c r="AD15" s="15">
         <v>5200</v>
       </c>
-      <c r="AC15" s="15">
+      <c r="AE15" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD15" s="15">
+      <c r="AF15" s="15">
         <v>140.4</v>
       </c>
-      <c r="AE15" s="15">
+      <c r="AG15" s="15">
         <v>410.8</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="28">
         <v>33</v>
       </c>
@@ -2806,43 +2887,45 @@
       <c r="T16" s="4">
         <v>270</v>
       </c>
-      <c r="U16" s="4">
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4">
         <v>42.1</v>
       </c>
-      <c r="V16" s="7">
+      <c r="X16" s="7">
         <v>2400</v>
       </c>
-      <c r="W16" s="7">
+      <c r="Y16" s="7">
         <v>3700</v>
       </c>
-      <c r="X16" s="14">
+      <c r="Z16" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y16" s="7">
+      <c r="AA16" s="7">
         <v>182.1</v>
       </c>
-      <c r="Z16" s="7">
+      <c r="AB16" s="7">
         <v>564.29999999999995</v>
       </c>
-      <c r="AA16" s="15">
+      <c r="AC16" s="15">
         <v>3600</v>
       </c>
-      <c r="AB16" s="15">
+      <c r="AD16" s="15">
         <v>5200</v>
       </c>
-      <c r="AC16" s="15">
+      <c r="AE16" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD16" s="15">
+      <c r="AF16" s="15">
         <v>148.6</v>
       </c>
-      <c r="AE16" s="15">
+      <c r="AG16" s="15">
         <v>431.2</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
         <v>36</v>
       </c>
@@ -2901,43 +2984,45 @@
       <c r="T17" s="4">
         <v>294</v>
       </c>
-      <c r="U17" s="4">
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4">
         <v>44.7</v>
       </c>
-      <c r="V17" s="7">
+      <c r="X17" s="7">
         <v>2400</v>
       </c>
-      <c r="W17" s="7">
+      <c r="Y17" s="7">
         <v>3700</v>
       </c>
-      <c r="X17" s="14">
+      <c r="Z17" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y17" s="7">
+      <c r="AA17" s="7">
         <v>194.1</v>
       </c>
-      <c r="Z17" s="7">
+      <c r="AB17" s="7">
         <v>603.6</v>
       </c>
-      <c r="AA17" s="15">
+      <c r="AC17" s="15">
         <v>3600</v>
       </c>
-      <c r="AB17" s="15">
+      <c r="AD17" s="15">
         <v>5200</v>
       </c>
-      <c r="AC17" s="15">
+      <c r="AE17" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD17" s="15">
+      <c r="AF17" s="15">
         <v>158.5</v>
       </c>
-      <c r="AE17" s="15">
+      <c r="AG17" s="15">
         <v>460.7</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
         <v>40</v>
       </c>
@@ -2996,43 +3081,45 @@
       <c r="T18" s="4">
         <v>326</v>
       </c>
-      <c r="U18" s="4">
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4">
         <v>47.1</v>
       </c>
-      <c r="V18" s="7">
+      <c r="X18" s="7">
         <v>2400</v>
       </c>
-      <c r="W18" s="7">
+      <c r="Y18" s="7">
         <v>3700</v>
       </c>
-      <c r="X18" s="14">
+      <c r="Z18" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y18" s="7">
+      <c r="AA18" s="7">
         <v>202.8</v>
       </c>
-      <c r="Z18" s="7">
+      <c r="AB18" s="7">
         <v>622.79999999999995</v>
       </c>
-      <c r="AA18" s="15">
+      <c r="AC18" s="15">
         <v>3600</v>
       </c>
-      <c r="AB18" s="15">
+      <c r="AD18" s="15">
         <v>5200</v>
       </c>
-      <c r="AC18" s="15">
+      <c r="AE18" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD18" s="15">
+      <c r="AF18" s="15">
         <v>165.6</v>
       </c>
-      <c r="AE18" s="15">
+      <c r="AG18" s="15">
         <v>478</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="28">
         <v>45</v>
       </c>
@@ -3091,43 +3178,45 @@
       <c r="T19" s="4">
         <v>365</v>
       </c>
-      <c r="U19" s="4">
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4">
         <v>49.4</v>
       </c>
-      <c r="V19" s="7">
+      <c r="X19" s="7">
         <v>2400</v>
       </c>
-      <c r="W19" s="7">
+      <c r="Y19" s="7">
         <v>3700</v>
       </c>
-      <c r="X19" s="14">
+      <c r="Z19" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y19" s="7">
+      <c r="AA19" s="7">
         <v>211.6</v>
       </c>
-      <c r="Z19" s="7">
+      <c r="AB19" s="7">
         <v>647.1</v>
       </c>
-      <c r="AA19" s="15">
+      <c r="AC19" s="15">
         <v>3600</v>
       </c>
-      <c r="AB19" s="15">
+      <c r="AD19" s="15">
         <v>5200</v>
       </c>
-      <c r="AC19" s="15">
+      <c r="AE19" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD19" s="15">
+      <c r="AF19" s="15">
         <v>172.8</v>
       </c>
-      <c r="AE19" s="15">
+      <c r="AG19" s="15">
         <v>498.4</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
         <v>50</v>
       </c>
@@ -3186,43 +3275,45 @@
       <c r="T20" s="4">
         <v>404</v>
       </c>
-      <c r="U20" s="4">
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4">
         <v>51.8</v>
       </c>
-      <c r="V20" s="7">
+      <c r="X20" s="7">
         <v>2400</v>
       </c>
-      <c r="W20" s="7">
+      <c r="Y20" s="7">
         <v>3700</v>
       </c>
-      <c r="X20" s="14">
+      <c r="Z20" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y20" s="7">
+      <c r="AA20" s="7">
         <v>220.4</v>
       </c>
-      <c r="Z20" s="7">
+      <c r="AB20" s="7">
         <v>676.1</v>
       </c>
-      <c r="AA20" s="15">
+      <c r="AC20" s="15">
         <v>3600</v>
       </c>
-      <c r="AB20" s="15">
+      <c r="AD20" s="15">
         <v>5200</v>
       </c>
-      <c r="AC20" s="15">
+      <c r="AE20" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD20" s="15">
+      <c r="AF20" s="15">
         <v>180</v>
       </c>
-      <c r="AE20" s="15">
+      <c r="AG20" s="15">
         <v>521.5</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="28">
         <v>55</v>
       </c>
@@ -3281,43 +3372,45 @@
       <c r="T21" s="4">
         <v>442</v>
       </c>
-      <c r="U21" s="4">
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4">
         <v>54</v>
       </c>
-      <c r="V21" s="7">
+      <c r="X21" s="7">
         <v>2400</v>
       </c>
-      <c r="W21" s="7">
+      <c r="Y21" s="7">
         <v>3700</v>
       </c>
-      <c r="X21" s="14">
+      <c r="Z21" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y21" s="7">
+      <c r="AA21" s="7">
         <v>229</v>
       </c>
-      <c r="Z21" s="7">
+      <c r="AB21" s="7">
         <v>699</v>
       </c>
-      <c r="AA21" s="15">
+      <c r="AC21" s="15">
         <v>3600</v>
       </c>
-      <c r="AB21" s="15">
+      <c r="AD21" s="15">
         <v>5200</v>
       </c>
-      <c r="AC21" s="15">
+      <c r="AE21" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD21" s="15">
+      <c r="AF21" s="15">
         <v>187</v>
       </c>
-      <c r="AE21" s="15">
+      <c r="AG21" s="15">
         <v>540.4</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="28">
         <v>60</v>
       </c>
@@ -3376,49 +3469,55 @@
       <c r="T22" s="4">
         <v>481</v>
       </c>
-      <c r="U22" s="4">
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4">
         <v>56.5</v>
       </c>
-      <c r="V22" s="7">
+      <c r="X22" s="7">
         <v>2400</v>
       </c>
-      <c r="W22" s="7">
+      <c r="Y22" s="7">
         <v>3700</v>
       </c>
-      <c r="X22" s="14">
+      <c r="Z22" s="14">
         <f t="shared" si="0"/>
         <v>2040000</v>
       </c>
-      <c r="Y22" s="7">
+      <c r="AA22" s="7">
         <v>239.2</v>
       </c>
-      <c r="Z22" s="7">
+      <c r="AB22" s="7">
         <v>736.2</v>
       </c>
-      <c r="AA22" s="15">
+      <c r="AC22" s="15">
         <v>3600</v>
       </c>
-      <c r="AB22" s="15">
+      <c r="AD22" s="15">
         <v>5200</v>
       </c>
-      <c r="AC22" s="15">
+      <c r="AE22" s="15">
         <f t="shared" si="1"/>
         <v>2040000</v>
       </c>
-      <c r="AD22" s="15">
+      <c r="AF22" s="15">
         <v>195.3</v>
       </c>
-      <c r="AE22" s="15">
+      <c r="AG22" s="15">
         <v>568.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="X4:AB4"/>
+    <mergeCell ref="AC4:AG4"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A12:B12"/>
@@ -3427,15 +3526,11 @@
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="V4:Z4"/>
-    <mergeCell ref="AA4:AE4"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3466,10 +3561,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
@@ -3554,8 +3649,8 @@
       <c r="AF1" s="25"/>
     </row>
     <row r="2" spans="1:32" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3648,8 +3743,8 @@
       </c>
     </row>
     <row r="3" spans="1:32" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
@@ -3764,20 +3859,20 @@
       <c r="T4" s="17"/>
       <c r="U4" s="17"/>
       <c r="V4" s="17"/>
-      <c r="W4" s="27" t="s">
+      <c r="W4" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27" t="s">
+      <c r="X4" s="29"/>
+      <c r="Y4" s="29"/>
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27"/>
-      <c r="AF4" s="27"/>
+      <c r="AC4" s="29"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
     </row>
     <row r="5" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
@@ -6035,18 +6130,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
     <mergeCell ref="W4:AA4"/>
     <mergeCell ref="AB4:AF4"/>
     <mergeCell ref="A23:B23"/>
@@ -6062,6 +6145,18 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6072,9 +6167,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90868E53-18F5-40B8-9504-75C70C3C5846}">
   <dimension ref="A1:AD28"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z5" sqref="Z5:AB28"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6092,10 +6187,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
@@ -6174,8 +6269,8 @@
       <c r="AD1" s="25"/>
     </row>
     <row r="2" spans="1:30" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
@@ -6262,8 +6357,8 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
@@ -6370,20 +6465,20 @@
       <c r="R4" s="16"/>
       <c r="S4" s="16"/>
       <c r="T4" s="16"/>
-      <c r="U4" s="27" t="s">
+      <c r="U4" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27" t="s">
+      <c r="V4" s="29"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="29"/>
+      <c r="Y4" s="29"/>
+      <c r="Z4" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="29"/>
+      <c r="AD4" s="29"/>
     </row>
     <row r="5" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
@@ -8595,18 +8690,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
@@ -8623,6 +8706,18 @@
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="Z4:AD4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8632,7 +8727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771E3DAC-FEB5-411B-B2E8-8D4F834D5B4C}">
   <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
@@ -8654,10 +8749,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
@@ -8748,8 +8843,8 @@
       <c r="AH1" s="25"/>
     </row>
     <row r="2" spans="1:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
@@ -8848,8 +8943,8 @@
       </c>
     </row>
     <row r="3" spans="1:34" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
@@ -8972,20 +9067,20 @@
       <c r="V4" s="26"/>
       <c r="W4" s="26"/>
       <c r="X4" s="26"/>
-      <c r="Y4" s="27" t="s">
+      <c r="Y4" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27" t="s">
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="29"/>
+      <c r="AD4" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="AE4" s="27"/>
-      <c r="AF4" s="27"/>
-      <c r="AG4" s="27"/>
-      <c r="AH4" s="27"/>
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="29"/>
+      <c r="AH4" s="29"/>
     </row>
     <row r="5" spans="1:34" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
@@ -11485,12 +11580,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="Y4:AC4"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -11503,16 +11602,12 @@
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="Y4:AC4"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>